<commit_message>
push to merge request
</commit_message>
<xml_diff>
--- a/output/product2.xlsx
+++ b/output/product2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,54 +478,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Watch Series 9 [GPS + Cellular 41mm] Smartwatch with Pink Aluminum Case with Pink Sport Band M/L. Fitness Tracker, ECG Apps, Always-On Retina Display</t>
+          <t>iPhone 15 Silicone Case with MagSafe - Winter Blue ​​​​​​​</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B0CSV945N2</t>
+          <t>B0CHX1652P</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sin Información</t>
+          <t>$49.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sin Información</t>
+          <t>$49.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sin Información</t>
+          <t>4.6 out of 5 stars</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Sin Información</t>
+          <t>518</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Apple-Cellular-Smartwatch-Aluminum-Fitness/dp/B0CSV945N2/ref=sr_1_1?dib=eyJ2IjoiMSJ9.sPPD18rPTjrcYprY9_mDTYNgfNSd_HsPxnt1lvRC3IRUAfGTwoSV37UbkPQ_6_Ms-plSA8C-ODendeZBDGBYnWAIPKjf8vXCHjsMQeZpvuh9JBnC40pZdXBlq2WzA3BkzuIg4zedKq1iitJAHAoCry_c_B26_AjRBY-HghSFIltErYu-7v5GjtACxNRvWY39CzO_W-NtwF35Q1UrfbhWjrHOFMw4ijB5u0auDEO34gk.sEOuDizMbOoqepId9OgKWP4SfW9jylYPnZFIdgLidQ4&amp;dib_tag=se&amp;keywords=apple+watch+series+9&amp;qid=1709628031&amp;sr=8-1</t>
+          <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToxMDg4ODcwMTgxNjM3MDY1OjE3MDk3Mjc5OTU6c3BfYXRmOjMwMDEwNTQ2MTAzMDQwMjo6MDo6&amp;url=%2FApple-iPhone-Silicone-Case-MagSafe%2Fdp%2FB0CHX1652P%2Fref%3Dsr_1_1_sspa%3Fdib%3DeyJ2IjoiMSJ9.qyh_pbIPVBxch9dd0Ix18WCWwT3gv1oE4dFE54aClru3yAF9CQMDr-Z6Rf_g5QahuK0qjdQk-GYxK6AWr2VifgxEnUyRQGCxMvZLu3IzVY_GD6B2fbnG7cJsXjhd7XEW7dbxJVeFdhjfwuU9n6hYmHGUJqCfIA_7zg0qzCSB5OSu6uZ4dAavpoH7yQYhX8UCpooSKlLD7PvccSMygfQu-FvDR8cnVT5cxfHxw6a_TXQ.VIOByNiwmgmOR11EGV5L_gEUHctL0gkY2PvxBb2FmRA%26dib_tag%3Dse%26keywords%3Diphone%2B15%26qid%3D1709727995%26sr%3D8-1-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9hdGY%26psc%3D1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/61ETcfPZFJL._AC_UY218_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/51XqsbKijCL._AC_UY218_.jpg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Watch Series 9 [GPS 45mm] Smartwatch with Silver Aluminum Case with Winter Blue Sport Loop. Fitness Tracker, Blood Oxygen &amp; ECG Apps, Always-On Retina Display, Carbon Neutral</t>
+          <t>iPhone 15 Clear Case with MagSafe ​​​​​​​</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>B0CHXDW29R</t>
+          <t>B0CHX1M27P</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -540,64 +540,316 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4.7 out of 5 stars</t>
+          <t>4.3 out of 5 stars</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>3,846</t>
+          <t>134</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Apple-Smartwatch-Aluminum-Fitness-Tracker/dp/B0CHXDW29R/ref=sr_1_2?dib=eyJ2IjoiMSJ9.sPPD18rPTjrcYprY9_mDTYNgfNSd_HsPxnt1lvRC3IRUAfGTwoSV37UbkPQ_6_Ms-plSA8C-ODendeZBDGBYnWAIPKjf8vXCHjsMQeZpvuh9JBnC40pZdXBlq2WzA3BkzuIg4zedKq1iitJAHAoCry_c_B26_AjRBY-HghSFIltErYu-7v5GjtACxNRvWY39CzO_W-NtwF35Q1UrfbhWjrHOFMw4ijB5u0auDEO34gk.sEOuDizMbOoqepId9OgKWP4SfW9jylYPnZFIdgLidQ4&amp;dib_tag=se&amp;keywords=apple+watch+series+9&amp;qid=1709628031&amp;sr=8-2</t>
+          <t>https://www.amazon.com/sspa/click?ie=UTF8&amp;spc=MToxMDg4ODcwMTgxNjM3MDY1OjE3MDk3Mjc5OTU6c3BfYXRmOjMwMDEwNTQ2MTAzMjkwMjo6MDo6&amp;url=%2FApple-iPhone-Clear-Case-MagSafe%2Fdp%2FB0CHX1M27P%2Fref%3Dsr_1_2_sspa%3Fdib%3DeyJ2IjoiMSJ9.qyh_pbIPVBxch9dd0Ix18WCWwT3gv1oE4dFE54aClru3yAF9CQMDr-Z6Rf_g5QahuK0qjdQk-GYxK6AWr2VifgxEnUyRQGCxMvZLu3IzVY_GD6B2fbnG7cJsXjhd7XEW7dbxJVeFdhjfwuU9n6hYmHGUJqCfIA_7zg0qzCSB5OSu6uZ4dAavpoH7yQYhX8UCpooSKlLD7PvccSMygfQu-FvDR8cnVT5cxfHxw6a_TXQ.VIOByNiwmgmOR11EGV5L_gEUHctL0gkY2PvxBb2FmRA%26dib_tag%3Dse%26keywords%3Diphone%2B15%26qid%3D1709727995%26sr%3D8-2-spons%26sp_csd%3Dd2lkZ2V0TmFtZT1zcF9hdGY%26psc%3D1</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/81OjeU5w-aL._AC_UY218_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/410mLbFKZRL._AC_UY218_.jpg</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2 Pack PC Case with Tempered Glass Screen Protector Compatible with Apple Watch Series 9 (2023) Series 8 Series 7 41mm, Ultra-Thin Scratch Resistant Cover for iWatch, 1 Black+1 Transparent</t>
+          <t>Kryptall 14 Pro Unlocked Cellular Phone, Purple, 128GB Memory Storage Capacity</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>B09L4Q43L9</t>
+          <t>B0CJ8B8XJT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$4.98</t>
+          <t>Sin Información</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>$4.98</t>
+          <t>Sin Información</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4.5 out of 5 stars</t>
+          <t>Sin Información</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>149,763</t>
+          <t>Sin Información</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Misxi-Compatible-Ultra-Thin-Protective-Transparent/dp/B09L4Q43L9/ref=sr_1_3?dib=eyJ2IjoiMSJ9.sPPD18rPTjrcYprY9_mDTYNgfNSd_HsPxnt1lvRC3IRUAfGTwoSV37UbkPQ_6_Ms-plSA8C-ODendeZBDGBYnWAIPKjf8vXCHjsMQeZpvuh9JBnC40pZdXBlq2WzA3BkzuIg4zedKq1iitJAHAoCry_c_B26_AjRBY-HghSFIltErYu-7v5GjtACxNRvWY39CzO_W-NtwF35Q1UrfbhWjrHOFMw4ijB5u0auDEO34gk.sEOuDizMbOoqepId9OgKWP4SfW9jylYPnZFIdgLidQ4&amp;dib_tag=se&amp;keywords=apple+watch+series+9&amp;qid=1709628031&amp;sr=8-3</t>
+          <t>https://www.amazon.com/Kryptall-Unlocked-Cellular-Storage-Capacity/dp/B0CJ8B8XJT/ref=sr_1_3?dib=eyJ2IjoiMSJ9.qyh_pbIPVBxch9dd0Ix18WCWwT3gv1oE4dFE54aClru3yAF9CQMDr-Z6Rf_g5QahuK0qjdQk-GYxK6AWr2VifgxEnUyRQGCxMvZLu3IzVY_GD6B2fbnG7cJsXjhd7XEW7dbxJVeFdhjfwuU9n6hYmHGUJqCfIA_7zg0qzCSB5OSu6uZ4dAavpoH7yQYhX8UCpooSKlLD7PvccSMygfQu-FvDR8cnVT5cxfHxw6a_TXQ.VIOByNiwmgmOR11EGV5L_gEUHctL0gkY2PvxBb2FmRA&amp;dib_tag=se&amp;keywords=iphone+15&amp;qid=1709727995&amp;sr=8-3</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/81-RDEIf2lL._AC_UY218_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/61RklF9NgpL._AC_UY218_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Galaxy S24+ Plus Cell Phone, 256GB AI Smartphone, Unlocked Android, 50MP Camera, Fastest Processor, Long Battery Life, US Version, 2024, Onyx Black</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B0CMDL3H3V</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$999.99</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$999.99</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>4.0 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>338</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/SAMSUNG-Smartphone-Unlocked-Android-Processor/dp/B0CMDL3H3V/ref=sr_1_4?dib=eyJ2IjoiMSJ9.qyh_pbIPVBxch9dd0Ix18WCWwT3gv1oE4dFE54aClru3yAF9CQMDr-Z6Rf_g5QahuK0qjdQk-GYxK6AWr2VifgxEnUyRQGCxMvZLu3IzVY_GD6B2fbnG7cJsXjhd7XEW7dbxJVeFdhjfwuU9n6hYmHGUJqCfIA_7zg0qzCSB5OSu6uZ4dAavpoH7yQYhX8UCpooSKlLD7PvccSMygfQu-FvDR8cnVT5cxfHxw6a_TXQ.VIOByNiwmgmOR11EGV5L_gEUHctL0gkY2PvxBb2FmRA&amp;dib_tag=se&amp;keywords=iphone+15&amp;qid=1709727995&amp;sr=8-4</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71NngboUC6L._AC_UY218_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>I15 Pro Max Smartphone Unlocked Cell Phone,Battery 6800mAh 6.8 HD Screen Unlocked Phone,6+256GB Android 13 with 128GB Memory Card,Dual SIM/5G/Fingerprint Lock/Face ID (Purple, 6+256)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B0CT63GF7X</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Sin Información</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sin Información</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>4.7 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Huness-Smartphone-Unlocked-Battery-Fingerprint/dp/B0CT63GF7X/ref=sr_1_5?dib=eyJ2IjoiMSJ9.qyh_pbIPVBxch9dd0Ix18WCWwT3gv1oE4dFE54aClru3yAF9CQMDr-Z6Rf_g5QahuK0qjdQk-GYxK6AWr2VifgxEnUyRQGCxMvZLu3IzVY_GD6B2fbnG7cJsXjhd7XEW7dbxJVeFdhjfwuU9n6hYmHGUJqCfIA_7zg0qzCSB5OSu6uZ4dAavpoH7yQYhX8UCpooSKlLD7PvccSMygfQu-FvDR8cnVT5cxfHxw6a_TXQ.VIOByNiwmgmOR11EGV5L_gEUHctL0gkY2PvxBb2FmRA&amp;dib_tag=se&amp;keywords=iphone+15&amp;qid=1709727995&amp;sr=8-5</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71UO5Rrpq-L._AC_UY218_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Galaxy S23 FE Cell Phone, 256GB, Unlocked Android Smartphone, Long Battery Life, Premium Processor, Tough Gorilla Glass Display, Hi-Res 50MP Camera, US Version, 2023, Cream</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>B0CD8YMKWC</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Sin Información</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sin Información</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>540</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/SAMSUNG-Unlocked-Android-Smartphone-Processor/dp/B0CD8YMKWC/ref=sr_1_6?dib=eyJ2IjoiMSJ9.qyh_pbIPVBxch9dd0Ix18WCWwT3gv1oE4dFE54aClru3yAF9CQMDr-Z6Rf_g5QahuK0qjdQk-GYxK6AWr2VifgxEnUyRQGCxMvZLu3IzVY_GD6B2fbnG7cJsXjhd7XEW7dbxJVeFdhjfwuU9n6hYmHGUJqCfIA_7zg0qzCSB5OSu6uZ4dAavpoH7yQYhX8UCpooSKlLD7PvccSMygfQu-FvDR8cnVT5cxfHxw6a_TXQ.VIOByNiwmgmOR11EGV5L_gEUHctL0gkY2PvxBb2FmRA&amp;dib_tag=se&amp;keywords=iphone+15&amp;qid=1709727995&amp;sr=8-6</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71ukK41npyL._AC_UY218_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>I15 PROMAX Unlocked Android Phone 2023 Android 13 Cell Phone with Dynamic Island Titanium Design 8GB+512GB Mobile Phones 6.7“ HD Screen 108MP+48MP Camera 6800 mAh Dual SIM Smart Phone (Blue)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>B0CP5K7ZZZ</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$199.99</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$199.99</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1.5 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Deeptick-Unlocked-Android-Dynamic-Titanium/dp/B0CP5K7ZZZ/ref=sr_1_7?dib=eyJ2IjoiMSJ9.qyh_pbIPVBxch9dd0Ix18WCWwT3gv1oE4dFE54aClru3yAF9CQMDr-Z6Rf_g5QahuK0qjdQk-GYxK6AWr2VifgxEnUyRQGCxMvZLu3IzVY_GD6B2fbnG7cJsXjhd7XEW7dbxJVeFdhjfwuU9n6hYmHGUJqCfIA_7zg0qzCSB5OSu6uZ4dAavpoH7yQYhX8UCpooSKlLD7PvccSMygfQu-FvDR8cnVT5cxfHxw6a_TXQ.VIOByNiwmgmOR11EGV5L_gEUHctL0gkY2PvxBb2FmRA&amp;dib_tag=se&amp;keywords=iphone+15&amp;qid=1709727995&amp;sr=8-7</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71v6aolL7qL._AC_UY218_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Open, 16GB RAM+512GB, Dual-SIM, Emerald Dusk, US Factory Unlocked Android Smartphone, 4805 mAh Battery, 67W Fast Charging, Hasselblad Camera, 120Hz Fluid Display</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>B0CHN8FNW3</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$1,699.99</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$1,699.99</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>4.0 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/OnePlus-Dual-SIM-Unlocked-Smartphone-Hasselblad/dp/B0CHN8FNW3/ref=sr_1_8?dib=eyJ2IjoiMSJ9.qyh_pbIPVBxch9dd0Ix18WCWwT3gv1oE4dFE54aClru3yAF9CQMDr-Z6Rf_g5QahuK0qjdQk-GYxK6AWr2VifgxEnUyRQGCxMvZLu3IzVY_GD6B2fbnG7cJsXjhd7XEW7dbxJVeFdhjfwuU9n6hYmHGUJqCfIA_7zg0qzCSB5OSu6uZ4dAavpoH7yQYhX8UCpooSKlLD7PvccSMygfQu-FvDR8cnVT5cxfHxw6a_TXQ.VIOByNiwmgmOR11EGV5L_gEUHctL0gkY2PvxBb2FmRA&amp;dib_tag=se&amp;keywords=iphone+15&amp;qid=1709727995&amp;sr=8-8</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61HbEkUjV-L._AC_UY218_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>A15 Pro Max Cell Phone,8GB+512GB Ultra Memory Unlocked Phone,Android 13.0 Smartphone,6800 mAh Battey,6.82-inch HD Screen,Dual SIM, Dual Standby,108MP Camera, 5G Phone.(Black)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>B0CR2TL446</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Sin Información</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Sin Información</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2.5 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/WV-LeisureMaster-A15-Smartphone-6-82-inch/dp/B0CR2TL446/ref=sr_1_9?dib=eyJ2IjoiMSJ9.qyh_pbIPVBxch9dd0Ix18WCWwT3gv1oE4dFE54aClru3yAF9CQMDr-Z6Rf_g5QahuK0qjdQk-GYxK6AWr2VifgxEnUyRQGCxMvZLu3IzVY_GD6B2fbnG7cJsXjhd7XEW7dbxJVeFdhjfwuU9n6hYmHGUJqCfIA_7zg0qzCSB5OSu6uZ4dAavpoH7yQYhX8UCpooSKlLD7PvccSMygfQu-FvDR8cnVT5cxfHxw6a_TXQ.VIOByNiwmgmOR11EGV5L_gEUHctL0gkY2PvxBb2FmRA&amp;dib_tag=se&amp;keywords=iphone+15&amp;qid=1709727995&amp;sr=8-9</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71aGs+ZlfML._AC_UY218_.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>